<commit_message>
Added Diffuser .dxf file
</commit_message>
<xml_diff>
--- a/Documentation/Revised_BOM.xlsx
+++ b/Documentation/Revised_BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theko_6tlzseu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theko_6tlzseu\Documents\Git\HyperShades\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA1C63C2-36DD-4295-9134-75E6CD094F84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021E3020-A859-409B-8CD7-48ACEC769391}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -232,16 +232,23 @@
   </si>
   <si>
     <t>Need to recheck pricing</t>
+  </si>
+  <si>
+    <t>Power Switch</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Toggle-Switches_Korean-Hroparts-Elec-K3-1260D-L1_C92657.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -274,8 +281,20 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,8 +313,14 @@
         <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -303,11 +328,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -320,11 +361,26 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -543,8 +599,8 @@
   </sheetPr>
   <dimension ref="A1:J1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -558,7 +614,7 @@
     <col min="10" max="10" width="21.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -860,7 +916,7 @@
         <v>0.03</v>
       </c>
       <c r="D12" s="5">
-        <f t="shared" ref="D12:D18" si="1">C12*B12</f>
+        <f t="shared" ref="D12:D17" si="1">C12*B12</f>
         <v>0.89999999999999991</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -974,7 +1030,7 @@
       </c>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>59</v>
       </c>
@@ -999,21 +1055,36 @@
       </c>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="11"/>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="15">
+        <v>10</v>
+      </c>
+      <c r="C18" s="16">
+        <v>0.11</v>
+      </c>
+      <c r="D18" s="16">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="14"/>
+      <c r="I18" s="18"/>
+    </row>
+    <row r="19" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="13"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="2" t="s">
         <v>63</v>
       </c>
@@ -1023,12 +1094,12 @@
     </row>
     <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="5">
-        <f>SUM(C2:C17)</f>
-        <v>7.4648128205128215</v>
+        <f>SUM(C2:C18)</f>
+        <v>7.5748128205128218</v>
       </c>
       <c r="D20" s="5">
         <f>SUM(D2:D18)</f>
-        <v>193.45976923076924</v>
+        <v>194.55976923076923</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="3" t="s">
@@ -1038,7 +1109,7 @@
     <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="I21" s="14"/>
+      <c r="I21" s="13"/>
       <c r="J21" s="3" t="s">
         <v>66</v>
       </c>
@@ -4997,7 +5068,9 @@
     <hyperlink ref="F15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="F16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="F17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F18" r:id="rId17" xr:uid="{B2ED0E9A-D8A8-4F64-BDB1-DA178FBE8D51}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>